<commit_message>
ADDED THE TABLE OF SERVER NAMES AND DATABASE NAMES
</commit_message>
<xml_diff>
--- a/dbms/lib/src/details.xlsx
+++ b/dbms/lib/src/details.xlsx
@@ -14,14 +14,11 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="67" uniqueCount="33">
   <si>
     <t>S.NO</t>
   </si>
   <si>
-    <t>SERVER</t>
-  </si>
-  <si>
     <t>MONGO</t>
   </si>
   <si>
@@ -32,6 +29,90 @@
   </si>
   <si>
     <t>MYSQL</t>
+  </si>
+  <si>
+    <t>TECHNOLOGY</t>
+  </si>
+  <si>
+    <t>SERVERNAME</t>
+  </si>
+  <si>
+    <t>a</t>
+  </si>
+  <si>
+    <t>b</t>
+  </si>
+  <si>
+    <t>c</t>
+  </si>
+  <si>
+    <t>d</t>
+  </si>
+  <si>
+    <t>db1</t>
+  </si>
+  <si>
+    <t>db2</t>
+  </si>
+  <si>
+    <t>db3</t>
+  </si>
+  <si>
+    <t>db4</t>
+  </si>
+  <si>
+    <t>db5</t>
+  </si>
+  <si>
+    <t>db6</t>
+  </si>
+  <si>
+    <t>db7</t>
+  </si>
+  <si>
+    <t>db8</t>
+  </si>
+  <si>
+    <t>db9</t>
+  </si>
+  <si>
+    <t>db10</t>
+  </si>
+  <si>
+    <t>db11</t>
+  </si>
+  <si>
+    <t>db12</t>
+  </si>
+  <si>
+    <t>db13</t>
+  </si>
+  <si>
+    <t>db14</t>
+  </si>
+  <si>
+    <t>db15</t>
+  </si>
+  <si>
+    <t>db16</t>
+  </si>
+  <si>
+    <t>db17</t>
+  </si>
+  <si>
+    <t>db18</t>
+  </si>
+  <si>
+    <t>db19</t>
+  </si>
+  <si>
+    <t>db20</t>
+  </si>
+  <si>
+    <t>db21</t>
+  </si>
+  <si>
+    <t>DATABASENAME</t>
   </si>
 </sst>
 </file>
@@ -67,8 +148,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -373,55 +457,329 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B5"/>
+  <dimension ref="A1:D22"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H11" sqref="H11"/>
+      <selection activeCell="D1" sqref="D1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="7.109375" customWidth="1"/>
+    <col min="2" max="2" width="24.6640625" customWidth="1"/>
+    <col min="3" max="3" width="23" customWidth="1"/>
+    <col min="4" max="4" width="21.21875" customWidth="1"/>
+    <col min="5" max="5" width="26.33203125" customWidth="1"/>
+    <col min="6" max="6" width="16.88671875" customWidth="1"/>
+    <col min="7" max="7" width="17.88671875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A1" t="s">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A2" s="1">
         <v>1</v>
       </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A2">
+      <c r="B2" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A3" s="1">
+        <v>2</v>
+      </c>
+      <c r="B3" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="B2" t="s">
+      <c r="C3" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A4" s="1">
+        <v>3</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A5" s="1">
+        <v>4</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A6" s="1">
         <v>5</v>
       </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A3">
+      <c r="B6" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="D6" s="1" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A7" s="1">
+        <v>6</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="D7" s="1" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A8" s="1">
+        <v>7</v>
+      </c>
+      <c r="B8" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="B3" t="s">
+      <c r="C8" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="D8" s="1" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A9" s="1">
+        <v>8</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C9" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="D9" s="1" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A10" s="1">
+        <v>9</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C10" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="D10" s="1" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A11" s="1">
+        <v>10</v>
+      </c>
+      <c r="B11" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C11" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="D11" s="1" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A12" s="1">
+        <v>11</v>
+      </c>
+      <c r="B12" s="1" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A4">
+      <c r="C12" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="D12" s="1" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A13" s="1">
+        <v>12</v>
+      </c>
+      <c r="B13" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="B4" t="s">
+      <c r="C13" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="D13" s="1" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A14" s="1">
+        <v>13</v>
+      </c>
+      <c r="B14" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C14" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="D14" s="1" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A15" s="1">
+        <v>14</v>
+      </c>
+      <c r="B15" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C15" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="D15" s="1" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A16" s="1">
+        <v>15</v>
+      </c>
+      <c r="B16" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C16" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="D16" s="1" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A17" s="1">
+        <v>16</v>
+      </c>
+      <c r="B17" s="1" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A5">
+      <c r="C17" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="D17" s="1" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A18" s="1">
+        <v>17</v>
+      </c>
+      <c r="B18" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="B5" t="s">
+      <c r="C18" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="D18" s="1" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A19" s="1">
+        <v>18</v>
+      </c>
+      <c r="B19" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C19" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="D19" s="1" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A20" s="1">
+        <v>19</v>
+      </c>
+      <c r="B20" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C20" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="D20" s="1" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A21" s="1">
+        <v>20</v>
+      </c>
+      <c r="B21" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C21" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="D21" s="1" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A22" s="1">
+        <v>21</v>
+      </c>
+      <c r="B22" s="1" t="s">
         <v>4</v>
+      </c>
+      <c r="C22" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="D22" s="1" t="s">
+        <v>31</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
MYSQL connection is made
</commit_message>
<xml_diff>
--- a/dbms/lib/src/details.xlsx
+++ b/dbms/lib/src/details.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="67" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="39">
   <si>
     <t>S.NO</t>
   </si>
@@ -49,9 +49,6 @@
     <t>d</t>
   </si>
   <si>
-    <t>db1</t>
-  </si>
-  <si>
     <t>db2</t>
   </si>
   <si>
@@ -113,6 +110,27 @@
   </si>
   <si>
     <t>DATABASENAME</t>
+  </si>
+  <si>
+    <t>PORTNO</t>
+  </si>
+  <si>
+    <t>HOSTNAME</t>
+  </si>
+  <si>
+    <t>TEST101</t>
+  </si>
+  <si>
+    <t>mydb1</t>
+  </si>
+  <si>
+    <t>127.0.0.1</t>
+  </si>
+  <si>
+    <t>USERNAME</t>
+  </si>
+  <si>
+    <t>root</t>
   </si>
 </sst>
 </file>
@@ -148,10 +166,13 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -457,10 +478,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D22"/>
+  <dimension ref="A1:G22"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D1" sqref="D1"/>
+    <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
+      <selection activeCell="G2" sqref="G2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -474,7 +495,7 @@
     <col min="7" max="7" width="17.88671875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -485,10 +506,19 @@
         <v>6</v>
       </c>
       <c r="D1" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="F1" s="1" t="s">
         <v>32</v>
       </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="G1" s="1" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A2" s="1">
         <v>1</v>
       </c>
@@ -496,13 +526,22 @@
         <v>4</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>7</v>
+        <v>34</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+        <v>35</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="F2" s="2">
+        <v>3306</v>
+      </c>
+      <c r="G2" s="1" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A3" s="1">
         <v>2</v>
       </c>
@@ -513,10 +552,10 @@
         <v>8</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A4" s="1">
         <v>3</v>
       </c>
@@ -527,10 +566,10 @@
         <v>9</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A5" s="1">
         <v>4</v>
       </c>
@@ -541,10 +580,10 @@
         <v>10</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A6" s="1">
         <v>5</v>
       </c>
@@ -555,10 +594,10 @@
         <v>7</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A7" s="1">
         <v>6</v>
       </c>
@@ -569,10 +608,10 @@
         <v>8</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A8" s="1">
         <v>7</v>
       </c>
@@ -583,10 +622,10 @@
         <v>9</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A9" s="1">
         <v>8</v>
       </c>
@@ -597,10 +636,10 @@
         <v>10</v>
       </c>
       <c r="D9" s="1" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A10" s="1">
         <v>9</v>
       </c>
@@ -611,10 +650,10 @@
         <v>7</v>
       </c>
       <c r="D10" s="1" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A11" s="1">
         <v>10</v>
       </c>
@@ -625,10 +664,10 @@
         <v>8</v>
       </c>
       <c r="D11" s="1" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A12" s="1">
         <v>11</v>
       </c>
@@ -639,10 +678,10 @@
         <v>9</v>
       </c>
       <c r="D12" s="1" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A13" s="1">
         <v>12</v>
       </c>
@@ -653,10 +692,10 @@
         <v>10</v>
       </c>
       <c r="D13" s="1" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.3">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A14" s="1">
         <v>13</v>
       </c>
@@ -667,10 +706,10 @@
         <v>7</v>
       </c>
       <c r="D14" s="1" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.3">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A15" s="1">
         <v>14</v>
       </c>
@@ -681,10 +720,10 @@
         <v>8</v>
       </c>
       <c r="D15" s="1" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.3">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A16" s="1">
         <v>15</v>
       </c>
@@ -695,7 +734,7 @@
         <v>9</v>
       </c>
       <c r="D16" s="1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.3">
@@ -709,7 +748,7 @@
         <v>10</v>
       </c>
       <c r="D17" s="1" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.3">
@@ -723,7 +762,7 @@
         <v>7</v>
       </c>
       <c r="D18" s="1" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.3">
@@ -737,7 +776,7 @@
         <v>8</v>
       </c>
       <c r="D19" s="1" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.3">
@@ -751,7 +790,7 @@
         <v>9</v>
       </c>
       <c r="D20" s="1" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.3">
@@ -765,7 +804,7 @@
         <v>10</v>
       </c>
       <c r="D21" s="1" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.3">
@@ -779,7 +818,7 @@
         <v>7</v>
       </c>
       <c r="D22" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
ADDED COLOR BUTTONS FOR THE TABLE
</commit_message>
<xml_diff>
--- a/dbms/lib/src/details.xlsx
+++ b/dbms/lib/src/details.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="94" uniqueCount="42">
   <si>
     <t>S.NO</t>
   </si>
@@ -131,6 +131,15 @@
   </si>
   <si>
     <t>root</t>
+  </si>
+  <si>
+    <t>CLR</t>
+  </si>
+  <si>
+    <t>r</t>
+  </si>
+  <si>
+    <t>g</t>
   </si>
 </sst>
 </file>
@@ -478,10 +487,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G22"/>
+  <dimension ref="A1:H22"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
-      <selection activeCell="G2" sqref="G2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G11" sqref="G11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -495,7 +504,7 @@
     <col min="7" max="7" width="17.88671875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -517,8 +526,11 @@
       <c r="G1" s="1" t="s">
         <v>37</v>
       </c>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H1" s="1" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A2" s="1">
         <v>1</v>
       </c>
@@ -540,8 +552,11 @@
       <c r="G2" s="1" t="s">
         <v>38</v>
       </c>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H2" s="1" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A3" s="1">
         <v>2</v>
       </c>
@@ -554,8 +569,11 @@
       <c r="D3" s="1" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H3" s="1" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A4" s="1">
         <v>3</v>
       </c>
@@ -568,8 +586,11 @@
       <c r="D4" s="1" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H4" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A5" s="1">
         <v>4</v>
       </c>
@@ -582,8 +603,11 @@
       <c r="D5" s="1" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H5" s="1" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A6" s="1">
         <v>5</v>
       </c>
@@ -596,8 +620,11 @@
       <c r="D6" s="1" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H6" s="1" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A7" s="1">
         <v>6</v>
       </c>
@@ -610,8 +637,11 @@
       <c r="D7" s="1" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H7" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A8" s="1">
         <v>7</v>
       </c>
@@ -624,8 +654,11 @@
       <c r="D8" s="1" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H8" s="1" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A9" s="1">
         <v>8</v>
       </c>
@@ -638,8 +671,11 @@
       <c r="D9" s="1" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H9" s="1" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A10" s="1">
         <v>9</v>
       </c>
@@ -652,8 +688,11 @@
       <c r="D10" s="1" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H10" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A11" s="1">
         <v>10</v>
       </c>
@@ -666,8 +705,11 @@
       <c r="D11" s="1" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H11" s="1" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A12" s="1">
         <v>11</v>
       </c>
@@ -680,8 +722,11 @@
       <c r="D12" s="1" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H12" s="1" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A13" s="1">
         <v>12</v>
       </c>
@@ -694,8 +739,11 @@
       <c r="D13" s="1" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H13" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A14" s="1">
         <v>13</v>
       </c>
@@ -708,8 +756,11 @@
       <c r="D14" s="1" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H14" s="1" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A15" s="1">
         <v>14</v>
       </c>
@@ -722,8 +773,11 @@
       <c r="D15" s="1" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H15" s="1" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A16" s="1">
         <v>15</v>
       </c>
@@ -736,8 +790,11 @@
       <c r="D16" s="1" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="H16" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A17" s="1">
         <v>16</v>
       </c>
@@ -750,8 +807,11 @@
       <c r="D17" s="1" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="H17" s="1" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A18" s="1">
         <v>17</v>
       </c>
@@ -764,8 +824,11 @@
       <c r="D18" s="1" t="s">
         <v>26</v>
       </c>
-    </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="H18" s="1" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="19" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A19" s="1">
         <v>18</v>
       </c>
@@ -778,8 +841,11 @@
       <c r="D19" s="1" t="s">
         <v>27</v>
       </c>
-    </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="H19" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="20" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A20" s="1">
         <v>19</v>
       </c>
@@ -792,8 +858,11 @@
       <c r="D20" s="1" t="s">
         <v>28</v>
       </c>
-    </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="H20" s="1" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="21" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A21" s="1">
         <v>20</v>
       </c>
@@ -806,8 +875,11 @@
       <c r="D21" s="1" t="s">
         <v>29</v>
       </c>
-    </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="H21" s="1" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="22" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A22" s="1">
         <v>21</v>
       </c>
@@ -819,6 +891,9 @@
       </c>
       <c r="D22" s="1" t="s">
         <v>30</v>
+      </c>
+      <c r="H22" s="1" t="s">
+        <v>8</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
ADDED AN EXTENSIVE PAGE FOR COLOR REVIEW IN THE MAIN TABLE
</commit_message>
<xml_diff>
--- a/dbms/lib/src/details.xlsx
+++ b/dbms/lib/src/details.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="94" uniqueCount="42">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="94" uniqueCount="43">
   <si>
     <t>S.NO</t>
   </si>
@@ -140,6 +140,9 @@
   </si>
   <si>
     <t>g</t>
+  </si>
+  <si>
+    <t>y</t>
   </si>
 </sst>
 </file>
@@ -490,7 +493,7 @@
   <dimension ref="A1:H22"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G11" sqref="G11"/>
+      <selection activeCell="H2" sqref="H2:H22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -587,7 +590,7 @@
         <v>12</v>
       </c>
       <c r="H4" s="1" t="s">
-        <v>8</v>
+        <v>42</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.3">
@@ -638,7 +641,7 @@
         <v>15</v>
       </c>
       <c r="H7" s="1" t="s">
-        <v>8</v>
+        <v>42</v>
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.3">
@@ -689,7 +692,7 @@
         <v>18</v>
       </c>
       <c r="H10" s="1" t="s">
-        <v>8</v>
+        <v>42</v>
       </c>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.3">
@@ -740,7 +743,7 @@
         <v>21</v>
       </c>
       <c r="H13" s="1" t="s">
-        <v>8</v>
+        <v>42</v>
       </c>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.3">
@@ -791,7 +794,7 @@
         <v>24</v>
       </c>
       <c r="H16" s="1" t="s">
-        <v>8</v>
+        <v>42</v>
       </c>
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.3">
@@ -842,7 +845,7 @@
         <v>27</v>
       </c>
       <c r="H19" s="1" t="s">
-        <v>8</v>
+        <v>42</v>
       </c>
     </row>
     <row r="20" spans="1:8" x14ac:dyDescent="0.3">
@@ -893,7 +896,7 @@
         <v>30</v>
       </c>
       <c r="H22" s="1" t="s">
-        <v>8</v>
+        <v>42</v>
       </c>
     </row>
   </sheetData>

</xml_diff>